<commit_message>
MODIF DU FICHIER LIMOGES
</commit_message>
<xml_diff>
--- a/BLOC NOTE/FICHIER TARIF CONSOMMABLE/Fichier clients pro Limoges.xlsx
+++ b/BLOC NOTE/FICHIER TARIF CONSOMMABLE/Fichier clients pro Limoges.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="855">
   <si>
     <t xml:space="preserve">Catégories</t>
   </si>
@@ -2636,10 +2636,13 @@
     <t xml:space="preserve">05 87 19 95 61 </t>
   </si>
   <si>
+    <t xml:space="preserve">Dépannage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depeaupte et Fils </t>
+  </si>
+  <si>
     <t xml:space="preserve">19 Rue Pierre Dac </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depeaupte et Fils </t>
   </si>
   <si>
     <t xml:space="preserve">05 55 50 36 30 </t>
@@ -8538,7 +8541,7 @@
         <v>851</v>
       </c>
       <c r="C271" s="16" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="D271" s="4" t="n">
         <v>87000</v>
@@ -8547,7 +8550,7 @@
         <v>14</v>
       </c>
       <c r="F271" s="16" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="56.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17481,7 +17484,7 @@
     <row r="1760" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1760" s="2"/>
       <c r="B1760" s="2" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C1760" s="2"/>
       <c r="E1760" s="9"/>

</xml_diff>